<commit_message>
optimize timer update fifo8 to fifo32
</commit_message>
<xml_diff>
--- a/001-data/related.xlsx
+++ b/001-data/related.xlsx
@@ -1,17 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="2715" windowWidth="17880" windowHeight="8715" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="自定义图形" sheetId="1" r:id="rId1"/>
     <sheet name="内存规划图" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="others" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A10:K39"/>
 </workbook>
 </file>
 
@@ -299,15 +300,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -361,8 +362,68 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>150556</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="图片 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="685800" y="342900"/>
+          <a:ext cx="5600700" cy="1350706"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -404,7 +465,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -439,7 +500,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1514,53 +1575,53 @@
   </cols>
   <sheetData>
     <row r="1" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F1" s="19"/>
+      <c r="F1" s="18"/>
     </row>
     <row r="2" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F2" s="18"/>
+      <c r="F2" s="17"/>
       <c r="G2" s="10" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="3" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F3" s="17"/>
+      <c r="F3" s="16"/>
       <c r="G3" s="9"/>
     </row>
     <row r="4" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F4" s="17"/>
+      <c r="F4" s="16"/>
       <c r="G4" s="9"/>
     </row>
     <row r="5" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F5" s="17"/>
+      <c r="F5" s="16"/>
       <c r="G5" s="7" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="6" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F6" s="16"/>
+      <c r="F6" s="15"/>
       <c r="G6" s="10" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="7" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F7" s="16"/>
+      <c r="F7" s="15"/>
       <c r="G7" s="9"/>
       <c r="H7" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="8" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F8" s="16"/>
+      <c r="F8" s="15"/>
       <c r="G8" s="9"/>
     </row>
     <row r="9" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F9" s="16"/>
+      <c r="F9" s="15"/>
       <c r="G9" s="7" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="10" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="14" t="s">
         <v>19</v>
       </c>
       <c r="G10" s="10" t="s">
@@ -1568,42 +1629,42 @@
       </c>
     </row>
     <row r="11" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F11" s="15"/>
+      <c r="F11" s="14"/>
       <c r="G11" s="9"/>
       <c r="H11" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="12" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F12" s="15"/>
+      <c r="F12" s="14"/>
       <c r="G12" s="9"/>
     </row>
     <row r="13" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="15"/>
+      <c r="F13" s="14"/>
       <c r="G13" s="7" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="14" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F14" s="14"/>
+      <c r="F14" s="13"/>
       <c r="G14" s="10" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="15" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F15" s="14"/>
+      <c r="F15" s="13"/>
       <c r="G15" s="9"/>
-      <c r="H15" s="13" t="s">
+      <c r="H15" s="19" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="16" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F16" s="14"/>
+      <c r="F16" s="13"/>
       <c r="G16" s="9"/>
-      <c r="H16" s="13"/>
+      <c r="H16" s="19"/>
     </row>
     <row r="17" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F17" s="14"/>
+      <c r="F17" s="13"/>
       <c r="G17" s="7" t="s">
         <v>13</v>
       </c>
@@ -1617,14 +1678,14 @@
     <row r="19" spans="6:8" x14ac:dyDescent="0.15">
       <c r="F19" s="12"/>
       <c r="G19" s="9"/>
-      <c r="H19" s="13" t="s">
+      <c r="H19" s="19" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="20" spans="6:8" x14ac:dyDescent="0.15">
       <c r="F20" s="12"/>
       <c r="G20" s="9"/>
-      <c r="H20" s="13"/>
+      <c r="H20" s="19"/>
     </row>
     <row r="21" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
       <c r="F21" s="12"/>
@@ -1690,13 +1751,18 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="C8"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData/>
+  <sheetData>
+    <row r="8" spans="3:3" x14ac:dyDescent="0.15"/>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
add ls,cls,and dir command
</commit_message>
<xml_diff>
--- a/001-data/related.xlsx
+++ b/001-data/related.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="2715" windowWidth="17880" windowHeight="8715" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17400" windowHeight="9855" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="自定义图形" sheetId="1" r:id="rId1"/>
@@ -63,59 +63,59 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>0x0027 0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0026 ffff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>256*8=2K,存放IDT表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0026 f800</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0026 f7ff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0026 8000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0026 7fff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1440k，保存软盘内容</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0010 0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x000f ffff</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0x0000 0000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>30K，空</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>8192*8=64K，存放GDT表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0027 0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0026 ffff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>256*8=2K,存放IDT表</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0026 f800</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0026 f7ff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>30K，空</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0026 8000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0026 7fff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>1440k，保存软盘内容</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0010 0000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x000f ffff</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0x0000 0000</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -204,7 +204,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -229,28 +229,6 @@
       </left>
       <right/>
       <top/>
-      <bottom style="medium">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color auto="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -276,11 +254,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -293,21 +284,24 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -423,7 +417,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题​​">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 主题">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -465,7 +459,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -500,7 +494,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1560,183 +1554,202 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="F1:H30"/>
+  <dimension ref="C1:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H19" sqref="H19:H20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="5" max="5" width="12.375" customWidth="1"/>
+    <col min="2" max="2" width="3.875" customWidth="1"/>
+    <col min="3" max="3" width="22" customWidth="1"/>
+    <col min="4" max="4" width="2.875" customWidth="1"/>
+    <col min="5" max="5" width="14.375" customWidth="1"/>
     <col min="6" max="6" width="9" style="5"/>
     <col min="7" max="7" width="14.25" style="4" customWidth="1"/>
     <col min="8" max="8" width="42.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F1" s="18"/>
-    </row>
-    <row r="2" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F2" s="17"/>
-      <c r="G2" s="10" t="s">
+    <row r="1" spans="3:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="F1" s="15"/>
+    </row>
+    <row r="2" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="E2" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="14"/>
+    </row>
+    <row r="3" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="E3" s="18"/>
+      <c r="F3" s="13"/>
+    </row>
+    <row r="4" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="E4" s="18"/>
+      <c r="F4" s="13"/>
+    </row>
+    <row r="5" spans="3:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="19" t="s">
+        <v>21</v>
+      </c>
+      <c r="F5" s="13"/>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="F6" s="12"/>
+      <c r="G6" s="17" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="F7" s="12"/>
+      <c r="G7" s="18"/>
+      <c r="H7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="F8" s="12"/>
+      <c r="G8" s="18"/>
+    </row>
+    <row r="9" spans="3:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="F9" s="12"/>
+      <c r="G9" s="19" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="E10" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="F10" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="C11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="E11" s="5"/>
+      <c r="F11" s="11"/>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="E12" s="5"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="7"/>
+    </row>
+    <row r="13" spans="3:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="E13" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="F13" s="11"/>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="F14" s="10"/>
+      <c r="G14" s="17" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="F15" s="10"/>
+      <c r="G15" s="18"/>
+      <c r="H15" s="16" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="F16" s="10"/>
+      <c r="G16" s="18"/>
+      <c r="H16" s="16"/>
+    </row>
+    <row r="17" spans="3:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="F17" s="10"/>
+      <c r="G17" s="19" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="E18" s="17" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="9"/>
+    </row>
+    <row r="19" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="C19" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="3" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F3" s="16"/>
-      <c r="G3" s="9"/>
-    </row>
-    <row r="4" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F4" s="16"/>
-      <c r="G4" s="9"/>
-    </row>
-    <row r="5" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F5" s="16"/>
-      <c r="G5" s="7" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F6" s="15"/>
-      <c r="G6" s="10" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F7" s="15"/>
-      <c r="G7" s="9"/>
-      <c r="H7" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="8" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F8" s="15"/>
-      <c r="G8" s="9"/>
-    </row>
-    <row r="9" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F9" s="15"/>
-      <c r="G9" s="7" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="10" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F10" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="10" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F11" s="14"/>
-      <c r="G11" s="9"/>
-      <c r="H11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F12" s="14"/>
-      <c r="G12" s="9"/>
-    </row>
-    <row r="13" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F13" s="14"/>
-      <c r="G13" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F14" s="13"/>
-      <c r="G14" s="10" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="15" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F15" s="13"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="19" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F16" s="13"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="19"/>
-    </row>
-    <row r="17" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F17" s="13"/>
-      <c r="G17" s="7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="18" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F18" s="12"/>
-      <c r="G18" s="10" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="19" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F19" s="12"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="19" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="20" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F20" s="12"/>
-      <c r="G20" s="9"/>
-      <c r="H20" s="19"/>
-    </row>
-    <row r="21" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F21" s="12"/>
-      <c r="G21" s="7" t="s">
+      <c r="E19" s="5"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="7"/>
+      <c r="H19" s="16"/>
+    </row>
+    <row r="20" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="E20" s="5"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="7"/>
+      <c r="H20" s="16"/>
+    </row>
+    <row r="21" spans="3:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="E21" s="19" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="22" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F22" s="11"/>
-      <c r="G22" s="10" t="s">
+      <c r="F21" s="9"/>
+    </row>
+    <row r="22" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="F22" s="8"/>
+      <c r="G22" s="17" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="23" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F23" s="11"/>
-      <c r="G23" s="9"/>
-    </row>
-    <row r="24" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F24" s="11"/>
-      <c r="G24" s="9"/>
-    </row>
-    <row r="25" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F25" s="11"/>
-      <c r="G25" s="7" t="s">
+    <row r="23" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="F23" s="8"/>
+      <c r="G23" s="18"/>
+    </row>
+    <row r="24" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="F24" s="8"/>
+      <c r="G24" s="18"/>
+    </row>
+    <row r="25" spans="3:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="F25" s="8"/>
+      <c r="G25" s="19" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F26" s="8"/>
-      <c r="G26" s="10" t="s">
+    <row r="26" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="E26" s="17" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="27" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F27" s="8"/>
-      <c r="G27" s="9"/>
-    </row>
-    <row r="28" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="F28" s="8"/>
-      <c r="G28" s="9"/>
-    </row>
-    <row r="29" spans="6:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
-      <c r="F29" s="8"/>
-      <c r="G29" s="7" t="s">
+      <c r="F26" s="6"/>
+    </row>
+    <row r="27" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="E27" s="5"/>
+      <c r="F27" s="6"/>
+      <c r="G27" s="7"/>
+    </row>
+    <row r="28" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="E28" s="5"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="7"/>
+    </row>
+    <row r="29" spans="3:8" ht="14.25" thickBot="1" x14ac:dyDescent="0.2">
+      <c r="E29" s="19" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="30" spans="6:8" x14ac:dyDescent="0.15">
-      <c r="G30" s="6" t="s">
+      <c r="F29" s="6"/>
+    </row>
+    <row r="30" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="G30" s="17" t="s">
         <v>5</v>
       </c>
+    </row>
+    <row r="31" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="G31" s="5"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.15">
+      <c r="G32" s="5"/>
+    </row>
+    <row r="33" spans="7:7" x14ac:dyDescent="0.15">
+      <c r="G33" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">

</xml_diff>